<commit_message>
update pre lec 1 FA19
</commit_message>
<xml_diff>
--- a/course_materials/Fall2019_StatComp_course_assessment_plan.xlsx
+++ b/course_materials/Fall2019_StatComp_course_assessment_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfred/OneDrive - University of Nevada, Reno/Teaching/STAT_445-645/git_public/course_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF97867-38CF-E34E-B046-453B775BA4CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F2E73E-606E-9C47-80B7-74A8D97492DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="34400" windowHeight="28240" xr2:uid="{817317F3-93E4-1348-8419-7945FAAB9BF9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" xr2:uid="{817317F3-93E4-1348-8419-7945FAAB9BF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
rename using 0 prefix for easier sorting
</commit_message>
<xml_diff>
--- a/course_materials/Fall2019_StatComp_course_assessment_plan.xlsx
+++ b/course_materials/Fall2019_StatComp_course_assessment_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfred/OneDrive - University of Nevada, Reno/Teaching/STAT_445-645/git_public/course_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F2E73E-606E-9C47-80B7-74A8D97492DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472C9850-A9CB-FA4D-9AF3-BF202592EC86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" xr2:uid="{817317F3-93E4-1348-8419-7945FAAB9BF9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="34400" windowHeight="28240" xr2:uid="{817317F3-93E4-1348-8419-7945FAAB9BF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -533,7 +533,7 @@
   <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1269,7 +1269,10 @@
         <f t="shared" si="1"/>
         <v>700</v>
       </c>
-      <c r="J29" s="4"/>
+      <c r="J29" s="4">
+        <f>I29/I29*100</f>
+        <v>100</v>
+      </c>
       <c r="K29" s="4"/>
     </row>
     <row r="30" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
show percentage SLO7 for 445
</commit_message>
<xml_diff>
--- a/course_materials/Fall2019_StatComp_course_assessment_plan.xlsx
+++ b/course_materials/Fall2019_StatComp_course_assessment_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfred/OneDrive - University of Nevada, Reno/Teaching/STAT_445-645/git_public/course_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472C9850-A9CB-FA4D-9AF3-BF202592EC86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F53590-D470-5B45-A181-F5C41CE38549}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="34400" windowHeight="28240" xr2:uid="{817317F3-93E4-1348-8419-7945FAAB9BF9}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1347,7 +1347,10 @@
         <f>(G29/(I29-I28))*100</f>
         <v>12.727272727272727</v>
       </c>
-      <c r="H31" s="4"/>
+      <c r="H31" s="4">
+        <f>H27/(I29-H28)*100</f>
+        <v>3.6363636363636362</v>
+      </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>

</xml_diff>